<commit_message>
closes #69; changes some other definitions but only to separate examples out
</commit_message>
<xml_diff>
--- a/classification-systems/nzlum/build/nzlum_v0.4.0.xlsx
+++ b/classification-systems/nzlum/build/nzlum_v0.4.0.xlsx
@@ -1854,40 +1854,40 @@
     <row r="78">
       <c r="A78" s="2" t="n"/>
       <c r="B78" s="2" t="n"/>
-      <c r="C78" s="2" t="inlineStr">
-        <is>
-          <t>3.6.0</t>
-        </is>
-      </c>
-      <c r="D78" s="2" t="inlineStr">
-        <is>
-          <t>Transport and communication</t>
-        </is>
-      </c>
+      <c r="C78" s="2" t="n"/>
+      <c r="D78" s="2" t="n"/>
       <c r="E78" s="2" t="inlineStr">
         <is>
-          <t>3.6.1</t>
+          <t>3.5.8</t>
         </is>
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>Airports/aerodromes</t>
+          <t>Navigation and communication</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n"/>
       <c r="B79" s="2" t="n"/>
-      <c r="C79" s="2" t="n"/>
-      <c r="D79" s="2" t="n"/>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
+          <t>3.6.0</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
-          <t>3.6.2</t>
+          <t>3.6.1</t>
         </is>
       </c>
       <c r="F79" s="2" t="inlineStr">
         <is>
-          <t>Roads</t>
+          <t>Airports/aerodromes</t>
         </is>
       </c>
     </row>
@@ -1898,12 +1898,12 @@
       <c r="D80" s="2" t="n"/>
       <c r="E80" s="2" t="inlineStr">
         <is>
-          <t>3.6.3</t>
+          <t>3.6.2</t>
         </is>
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>Railways</t>
+          <t>Roads</t>
         </is>
       </c>
     </row>
@@ -1914,12 +1914,12 @@
       <c r="D81" s="2" t="n"/>
       <c r="E81" s="2" t="inlineStr">
         <is>
-          <t>3.6.4</t>
+          <t>3.6.3</t>
         </is>
       </c>
       <c r="F81" s="2" t="inlineStr">
         <is>
-          <t>Ports and water transport</t>
+          <t>Railways</t>
         </is>
       </c>
     </row>
@@ -1930,12 +1930,12 @@
       <c r="D82" s="2" t="n"/>
       <c r="E82" s="2" t="inlineStr">
         <is>
-          <t>3.6.5</t>
+          <t>3.6.4</t>
         </is>
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>Navigation and communication</t>
+          <t>Ports and water transport</t>
         </is>
       </c>
     </row>
@@ -2176,7 +2176,6 @@
     <mergeCell ref="C56:C58"/>
     <mergeCell ref="D56:D58"/>
     <mergeCell ref="D22:D25"/>
-    <mergeCell ref="C71:C77"/>
     <mergeCell ref="B52:B95"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C43:C47"/>
@@ -2186,11 +2185,11 @@
     <mergeCell ref="D93:D95"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="D59:D64"/>
+    <mergeCell ref="C79:C82"/>
     <mergeCell ref="B22:B51"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="D43:D47"/>
     <mergeCell ref="D65:D70"/>
-    <mergeCell ref="D71:D77"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="D52:D55"/>
     <mergeCell ref="D83:D87"/>
@@ -2204,9 +2203,9 @@
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="C59:C64"/>
     <mergeCell ref="D88:D92"/>
-    <mergeCell ref="C78:C82"/>
     <mergeCell ref="C52:C55"/>
     <mergeCell ref="C12:C19"/>
+    <mergeCell ref="C71:C78"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="C83:C87"/>
     <mergeCell ref="C93:C95"/>
@@ -2216,10 +2215,11 @@
     <mergeCell ref="A52:A95"/>
     <mergeCell ref="A22:A51"/>
     <mergeCell ref="D12:D19"/>
+    <mergeCell ref="D79:D82"/>
     <mergeCell ref="D29:D32"/>
+    <mergeCell ref="D71:D78"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="B2:B21"/>
-    <mergeCell ref="D78:D82"/>
     <mergeCell ref="C9:C11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>